<commit_message>
write on excel file
</commit_message>
<xml_diff>
--- a/src/test/java/recources/Capitals.xlsx
+++ b/src/test/java/recources/Capitals.xlsx
@@ -2,16 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -77,12 +79,25 @@
   </si>
   <si>
     <t>Oslo</t>
+  </si>
+  <si>
+    <t>POPULATION</t>
+  </si>
+  <si>
+    <t>150000</t>
+  </si>
+  <si>
+    <t>250000</t>
+  </si>
+  <si>
+    <t>54000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="10.0"/>
@@ -335,6 +350,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -347,6 +363,9 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -355,6 +374,9 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s" s="0">
+        <v>23</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -363,6 +385,9 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s" s="0">
+        <v>24</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
@@ -370,6 +395,9 @@
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
     <row r="5">

</xml_diff>